<commit_message>
some changes in git_memo. add readme.md
</commit_message>
<xml_diff>
--- a/GIT_memo.xlsx
+++ b/GIT_memo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="183">
   <si>
     <t>Настройка GIT</t>
   </si>
@@ -196,9 +196,6 @@
   </si>
   <si>
     <t>Удаление директории</t>
-  </si>
-  <si>
-    <t>rm Directory</t>
   </si>
   <si>
     <t>R</t>
@@ -650,6 +647,36 @@
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>GIT. Публикация</t>
+  </si>
+  <si>
+    <t>GIT. Настройка SSH подлючения</t>
+  </si>
+  <si>
+    <t>Примечание: SSH подключение - настройка уникального ключа</t>
+  </si>
+  <si>
+    <t>Генерация ключа</t>
+  </si>
+  <si>
+    <t>ssh-keygen</t>
+  </si>
+  <si>
+    <t>Генерирует файл с уникальным ключем. Как правило в папке пользователя. Переходим на сайт GitHub в меню Пользователь - Settings - SSH and GPG keys. Жмем кнопку New SSH key. Title записываем название ключа. Например: my computer. В поле Key скопировать содержимое файла-ключа. Жмем Add SSH key. Подтверждаем пароль.</t>
+  </si>
+  <si>
+    <t>Клонирование репозитория на компьютер</t>
+  </si>
+  <si>
+    <t>git clone &lt;ssh connection from GitHub&gt; &lt;Directory&gt;</t>
+  </si>
+  <si>
+    <t>Загружает проект с удаленного репозитор я по SSH подключению</t>
+  </si>
+  <si>
+    <t>rm -R Directory</t>
   </si>
 </sst>
 </file>
@@ -737,7 +764,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -772,6 +799,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -1074,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B73" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,110 +1264,110 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="C19" s="7"/>
       <c r="D19" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>68</v>
-      </c>
       <c r="C20" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="D22" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="C23" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="D23" s="10" t="s">
         <v>79</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="D24" s="10" t="s">
         <v>82</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="C25" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="C26" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1462,7 +1505,7 @@
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1470,18 +1513,18 @@
         <v>59</v>
       </c>
       <c r="B39" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="D39" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1489,17 +1532,17 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1518,58 +1561,58 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" s="11" t="s">
         <v>98</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>99</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>101</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>102</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>104</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>105</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="10"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1588,95 +1631,95 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B59" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="B59" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B61" s="11" t="s">
         <v>117</v>
-      </c>
-      <c r="B61" s="11" t="s">
-        <v>118</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D63" s="10" t="s">
         <v>123</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D64" s="10" t="s">
         <v>128</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1695,31 +1738,31 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B70" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="B70" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1738,81 +1781,81 @@
     </row>
     <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B75" s="11" t="s">
         <v>138</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>139</v>
       </c>
       <c r="C75" s="7"/>
       <c r="D75" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D76" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="B76" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D76" s="10" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B78" s="11" t="s">
         <v>148</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>149</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -1820,7 +1863,7 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1839,64 +1882,155 @@
     </row>
     <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B87" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="B87" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B88" s="11" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B89" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="B89" s="11" t="s">
-        <v>165</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B90" s="11" t="s">
         <v>167</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>168</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D91" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="B91" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C91" s="7" t="s">
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="12"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="12"/>
+      <c r="D92" s="14"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B93" s="13"/>
+      <c r="C93" s="12"/>
+      <c r="D93" s="14"/>
+    </row>
+    <row r="94" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
+      <c r="B94" s="15"/>
+      <c r="C94" s="15"/>
+      <c r="D94" s="16"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B95" s="13"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="14"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="12"/>
+      <c r="B96" s="13"/>
+      <c r="C96" s="12"/>
+      <c r="D96" s="14"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C98" s="7"/>
+      <c r="D98" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="D91" s="10" t="s">
-        <v>171</v>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B103" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="C103" s="7"/>
+      <c r="D103" s="10" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new changes rebase add
</commit_message>
<xml_diff>
--- a/GIT_memo.xlsx
+++ b/GIT_memo.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="17955"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Основная" sheetId="1" r:id="rId1"/>
+    <sheet name="Иллюстрации" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="211">
   <si>
     <t>Настройка GIT</t>
   </si>
@@ -738,7 +738,43 @@
     <t>git merge &lt;branch&gt;</t>
   </si>
   <si>
-    <t>Перед данной командой обязательно переключиться на ветку master.</t>
+    <t>Перед данной командой обязательно переключиться на ветку master. После слияния обязательно выполнить команду git push, чтобы загрузить изменения в удаленный репозиторий</t>
+  </si>
+  <si>
+    <t>Удаление веток</t>
+  </si>
+  <si>
+    <t>git branch -d &lt;branch&gt;</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Удаление веток. После ключа -d можно перечислить через пробел ветки, которые необходимо удалить.</t>
+  </si>
+  <si>
+    <t>Удаление веток в удаленном репозитории</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git push --delete origin &lt;branch&gt; </t>
+  </si>
+  <si>
+    <t>Удаление веток из удаленного репозитория</t>
+  </si>
+  <si>
+    <t>Перенос изменения ветки</t>
+  </si>
+  <si>
+    <t>Rebase - это операция смены старта ветки. Перемещает мои изменения в тот или иной момент времени.</t>
+  </si>
+  <si>
+    <t>Добавление всех файлов индекс для commit</t>
+  </si>
+  <si>
+    <t>git add .</t>
+  </si>
+  <si>
+    <t>Добавляет все файлы в индекс изменений</t>
   </si>
 </sst>
 </file>
@@ -893,6 +929,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="95250" y="542925"/>
+          <a:ext cx="8915400" cy="5305425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1182,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D112"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C94" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,473 +1804,523 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>110</v>
+        <v>208</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="10" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" s="10" t="s">
         <v>121</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B63" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B64" s="11" t="s">
+      <c r="B65" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C65" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D64" s="10" t="s">
+      <c r="D65" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B69" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C69" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D69" s="9" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B69" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="10" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B71" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" s="7"/>
+      <c r="D71" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B75" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C75" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D75" s="9" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C75" s="7"/>
-      <c r="D75" s="10" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B76" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" s="7"/>
+      <c r="D76" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="B76" s="11" t="s">
+      <c r="B77" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C77" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="D76" s="10" t="s">
+      <c r="D77" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="B78" s="11" t="s">
         <v>144</v>
-      </c>
-      <c r="C77" s="7"/>
-      <c r="D77" s="10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="B78" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="10" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B80" s="11" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="C80" s="7"/>
       <c r="D80" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B81" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C81" s="7"/>
+      <c r="D81" s="10" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="5"/>
-    </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+      <c r="A84" s="5"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="6" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B86" s="6" t="s">
+      <c r="B87" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C86" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D86" s="9" t="s">
+      <c r="D87" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B87" s="11" t="s">
+      <c r="B88" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="C87" s="7"/>
-      <c r="D87" s="10" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B88" s="11" t="s">
-        <v>161</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B89" s="11" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="10" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="10" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91" s="7"/>
+      <c r="D91" s="10" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="7" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B91" s="11" t="s">
+      <c r="B92" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C92" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="D91" s="10" t="s">
+      <c r="D92" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="12"/>
-      <c r="B92" s="13"/>
-      <c r="C92" s="12"/>
-      <c r="D92" s="14"/>
-    </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>174</v>
-      </c>
+      <c r="A93" s="12"/>
       <c r="B93" s="13"/>
       <c r="C93" s="12"/>
       <c r="D93" s="14"/>
     </row>
-    <row r="94" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="4"/>
-      <c r="B94" s="15"/>
-      <c r="C94" s="15"/>
-      <c r="D94" s="16"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" s="13"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="14"/>
+    </row>
+    <row r="95" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
+      <c r="B95" s="15"/>
+      <c r="C95" s="15"/>
+      <c r="D95" s="16"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B95" s="13"/>
-      <c r="C95" s="12"/>
-      <c r="D95" s="14"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="12"/>
       <c r="B96" s="13"/>
       <c r="C96" s="12"/>
       <c r="D96" s="14"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="6" t="s">
+      <c r="A97" s="12"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="12"/>
+      <c r="D97" s="14"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B97" s="6" t="s">
+      <c r="B98" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C97" s="6" t="s">
+      <c r="C98" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D97" s="9" t="s">
+      <c r="D98" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
+    <row r="99" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A99" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="B98" s="11" t="s">
+      <c r="B99" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C98" s="7"/>
-      <c r="D98" s="10" t="s">
+      <c r="C99" s="7"/>
+      <c r="D99" s="10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="6" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="6" t="s">
+      <c r="B103" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C102" s="6" t="s">
+      <c r="C103" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D102" s="9" t="s">
+      <c r="D103" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="7" t="s">
+    <row r="104" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B103" s="11" t="s">
+      <c r="B104" s="11" t="s">
         <v>180</v>
-      </c>
-      <c r="C103" s="7"/>
-      <c r="D103" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="B104" s="11" t="s">
-        <v>184</v>
       </c>
       <c r="C104" s="7"/>
       <c r="D104" s="10" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="B105" s="18" t="s">
-        <v>187</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A105" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>184</v>
       </c>
       <c r="C105" s="7"/>
       <c r="D105" s="10" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B107" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="C107" s="7"/>
+      <c r="D107" s="10" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="6" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B110" s="6" t="s">
+      <c r="B111" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="C111" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D110" s="9" t="s">
+      <c r="D111" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A111" s="7" t="s">
+    <row r="112" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A112" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B111" s="11" t="s">
+      <c r="B112" s="11" t="s">
         <v>195</v>
-      </c>
-      <c r="C111" s="7"/>
-      <c r="D111" s="10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>197</v>
       </c>
       <c r="C112" s="7"/>
       <c r="D112" s="10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A113" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B113" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C113" s="7"/>
+      <c r="D113" s="10" t="s">
         <v>198</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A114" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B114" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B115" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C115" s="7"/>
+      <c r="D115" s="10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A116" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B116" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="C116" s="7"/>
+      <c r="D116" s="10" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
@@ -2190,11 +2336,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>